<commit_message>
30-07-2018 : Added GlobalExculde in clsGlobals.cs, frmOtherConfig Two New Fields Added ->MastEmp->SPLALL,BAALL Changes in Accordance in frmEmployeeImport frmMastEmpBasicData frmMastEmpBulkChanges BugFixed : frmDomainConfig
</commit_message>
<xml_diff>
--- a/upload_template/EmpMasterChange_Upload.xlsx
+++ b/upload_template/EmpMasterChange_Upload.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="56">
   <si>
     <t>EmpUnqID</t>
   </si>
@@ -179,6 +179,15 @@
   </si>
   <si>
     <t>20053484</t>
+  </si>
+  <si>
+    <t>SPLALL</t>
+  </si>
+  <si>
+    <t>BAALL</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
@@ -248,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -256,6 +265,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -603,7 +614,7 @@
     <col min="5" max="5" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -619,8 +630,14 @@
       <c r="E1" s="3" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
@@ -636,8 +653,14 @@
       <c r="E2" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -653,8 +676,14 @@
       <c r="E3" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -670,8 +699,14 @@
       <c r="E4" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>45</v>
       </c>
@@ -687,8 +722,14 @@
       <c r="E5" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>46</v>
       </c>
@@ -704,8 +745,14 @@
       <c r="E6" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>48</v>
       </c>
@@ -721,8 +768,14 @@
       <c r="E7" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>49</v>
       </c>
@@ -738,8 +791,14 @@
       <c r="E8" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>50</v>
       </c>
@@ -755,8 +814,14 @@
       <c r="E9" s="4" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>51</v>
       </c>
@@ -772,8 +837,14 @@
       <c r="E10" s="4" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>52</v>
       </c>
@@ -788,6 +859,12 @@
       </c>
       <c r="E11" s="4" t="s">
         <v>47</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
24-08-2018 : BugFixed : LeaveEntry,Manual Sanction and Others
</commit_message>
<xml_diff>
--- a/upload_template/EmpMasterChange_Upload.xlsx
+++ b/upload_template/EmpMasterChange_Upload.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="57">
   <si>
     <t>EmpUnqID</t>
   </si>
@@ -188,6 +188,9 @@
   </si>
   <si>
     <t>0</t>
+  </si>
+  <si>
+    <t>LeftDt</t>
   </si>
 </sst>
 </file>
@@ -599,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,7 +617,7 @@
     <col min="5" max="5" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -636,8 +639,11 @@
       <c r="G1" s="5" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
@@ -660,7 +666,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -683,7 +689,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>44</v>
       </c>
@@ -706,7 +712,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>45</v>
       </c>
@@ -729,7 +735,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>46</v>
       </c>
@@ -752,7 +758,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>48</v>
       </c>
@@ -775,7 +781,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>49</v>
       </c>
@@ -798,7 +804,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>50</v>
       </c>
@@ -821,7 +827,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>51</v>
       </c>
@@ -844,7 +850,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>52</v>
       </c>

</xml_diff>

<commit_message>
2020-02-20 : Emp Address Details Upload combined in bulk employee change
</commit_message>
<xml_diff>
--- a/upload_template/EmpMasterChange_Upload.xlsx
+++ b/upload_template/EmpMasterChange_Upload.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22325"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SourceCode\Visual Studio 2013\Attendance\upload_template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SourceCode\Visual Studio 2013\Attendance - Indore\upload_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B61AFB27-37DF-4924-A90B-4BF4BF6C370F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8445" tabRatio="260"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
   <si>
     <t>EmpUnqID</t>
   </si>
@@ -154,33 +155,6 @@
     <t>20052833</t>
   </si>
   <si>
-    <t>20053169</t>
-  </si>
-  <si>
-    <t>20053316</t>
-  </si>
-  <si>
-    <t>20053447</t>
-  </si>
-  <si>
-    <t>314.3</t>
-  </si>
-  <si>
-    <t>20053454</t>
-  </si>
-  <si>
-    <t>20053458</t>
-  </si>
-  <si>
-    <t>20053464</t>
-  </si>
-  <si>
-    <t>20053481</t>
-  </si>
-  <si>
-    <t>20053484</t>
-  </si>
-  <si>
     <t>SPLALL</t>
   </si>
   <si>
@@ -191,13 +165,85 @@
   </si>
   <si>
     <t>LeftDt</t>
+  </si>
+  <si>
+    <t>BANKNAME</t>
+  </si>
+  <si>
+    <t>IFSCCODE</t>
+  </si>
+  <si>
+    <t>ACCOUNTNO</t>
+  </si>
+  <si>
+    <t>PANCARD</t>
+  </si>
+  <si>
+    <t>UANNO</t>
+  </si>
+  <si>
+    <t>MobileNo</t>
+  </si>
+  <si>
+    <t>EmailID</t>
+  </si>
+  <si>
+    <t>BloodGroup</t>
+  </si>
+  <si>
+    <t>PermenantAdd1</t>
+  </si>
+  <si>
+    <t>PermenantAdd2</t>
+  </si>
+  <si>
+    <t>PermenantAdd3</t>
+  </si>
+  <si>
+    <t>PermenantAdd4</t>
+  </si>
+  <si>
+    <t>PermenantDistrict</t>
+  </si>
+  <si>
+    <t>PermenantCity</t>
+  </si>
+  <si>
+    <t>PermenantState</t>
+  </si>
+  <si>
+    <t>PermenantPinCode</t>
+  </si>
+  <si>
+    <t>PresantAdd1</t>
+  </si>
+  <si>
+    <t>PresantAdd2</t>
+  </si>
+  <si>
+    <t>PresantAdd3</t>
+  </si>
+  <si>
+    <t>PresantAdd4</t>
+  </si>
+  <si>
+    <t>PresantDistrict</t>
+  </si>
+  <si>
+    <t>PresantCity</t>
+  </si>
+  <si>
+    <t>PresantState</t>
+  </si>
+  <si>
+    <t>PresantPinCode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,6 +254,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -233,7 +285,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -256,11 +308,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -270,6 +333,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -299,7 +365,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -391,6 +457,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -426,6 +509,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -601,11 +701,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -615,9 +715,21 @@
     <col min="3" max="3" width="15.28515625" style="4" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="9.140625" style="4"/>
+    <col min="9" max="9" width="13.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="16" width="18.42578125" customWidth="1"/>
+    <col min="17" max="18" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="28" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -634,16 +746,88 @@
         <v>38</v>
       </c>
       <c r="F1" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="O1" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="P1" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q1" s="9" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="R1" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="S1" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="T1" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="U1" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="V1" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="W1" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="X1" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y1" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z1" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA1" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AB1" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC1" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AD1" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE1" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF1" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
@@ -660,13 +844,16 @@
         <v>42</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="J2" s="7"/>
+      <c r="K2" s="7"/>
+      <c r="L2" s="7"/>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>43</v>
       </c>
@@ -683,194 +870,10 @@
         <v>42</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -880,7 +883,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AP41"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>